<commit_message>
Informações sobre as colunas e ideias para o projeto
</commit_message>
<xml_diff>
--- a/Projeto Final - Entrega 1.xlsx
+++ b/Projeto Final - Entrega 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavio\Dropbox\My PC (LAPTOP-FVTATBSD)\Documents\Pós Insper Data Science\AEM II\Projeto Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C98F88B-841B-4A50-A4D9-D7D176A7CD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC33597-27FC-427D-B6F5-7ECA5558D5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38578D12-16BC-486B-9148-65477D577933}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="131">
   <si>
     <t>Nome da base de dados</t>
   </si>
@@ -98,15 +98,9 @@
     <t>Prever o score da avaliação do café (total_cup_points) a partir das demais preditoras do dataset e agrupar os tipos de café (cluster)</t>
   </si>
   <si>
-    <t>double</t>
-  </si>
-  <si>
     <t>species</t>
   </si>
   <si>
-    <t>character</t>
-  </si>
-  <si>
     <t>owner</t>
   </si>
   <si>
@@ -231,6 +225,210 @@
   </si>
   <si>
     <t>total_cup_points</t>
+  </si>
+  <si>
+    <t>dbl</t>
+  </si>
+  <si>
+    <t>chr</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Total rating/points (0 - 100 scale)</t>
+  </si>
+  <si>
+    <t>Species of coffee bean (arabica or robusta)</t>
+  </si>
+  <si>
+    <t>Owner of the farm</t>
+  </si>
+  <si>
+    <t>Where the bean came from</t>
+  </si>
+  <si>
+    <t>Name of the farm</t>
+  </si>
+  <si>
+    <t>Lot number of the beans tested</t>
+  </si>
+  <si>
+    <t>Mill where the beans were processed</t>
+  </si>
+  <si>
+    <t>International Coffee Organization number</t>
+  </si>
+  <si>
+    <t>Company name</t>
+  </si>
+  <si>
+    <t>Altitude - this is a messy column - I've left it for some cleaning</t>
+  </si>
+  <si>
+    <t>Region where bean came from</t>
+  </si>
+  <si>
+    <t>Producer of the roasted bean</t>
+  </si>
+  <si>
+    <t>Number of bags tested</t>
+  </si>
+  <si>
+    <t>Bag weight tested</t>
+  </si>
+  <si>
+    <t>Partner for the country</t>
+  </si>
+  <si>
+    <t>When the beans were harvested (year)</t>
+  </si>
+  <si>
+    <t>When the beans were graded</t>
+  </si>
+  <si>
+    <t>Who owns the beans</t>
+  </si>
+  <si>
+    <t>Variety of the beans</t>
+  </si>
+  <si>
+    <t>Method for processing</t>
+  </si>
+  <si>
+    <t>Aroma grade</t>
+  </si>
+  <si>
+    <t>Flavor grade</t>
+  </si>
+  <si>
+    <t>Aftertaste grade</t>
+  </si>
+  <si>
+    <t>Acidity grade</t>
+  </si>
+  <si>
+    <t>Body grade</t>
+  </si>
+  <si>
+    <t>Balance grade</t>
+  </si>
+  <si>
+    <t>Uniformity grade</t>
+  </si>
+  <si>
+    <t>Clean cup grade</t>
+  </si>
+  <si>
+    <t>Sweetness grade</t>
+  </si>
+  <si>
+    <t>Cupper Points</t>
+  </si>
+  <si>
+    <t>Moisture Grade</t>
+  </si>
+  <si>
+    <t>Category one defects (count)</t>
+  </si>
+  <si>
+    <t>Color of bean</t>
+  </si>
+  <si>
+    <t>Category two defects (count)</t>
+  </si>
+  <si>
+    <t>Expiration date of the beans</t>
+  </si>
+  <si>
+    <t>Who certified it</t>
+  </si>
+  <si>
+    <t>Certification body address</t>
+  </si>
+  <si>
+    <t>Certification contact</t>
+  </si>
+  <si>
+    <t>Unit of measurement</t>
+  </si>
+  <si>
+    <t>Altitude low meters</t>
+  </si>
+  <si>
+    <t>Altitude high meters</t>
+  </si>
+  <si>
+    <t>Altitude mean meters</t>
+  </si>
+  <si>
+    <t>Variável que será prevista</t>
+  </si>
+  <si>
+    <t>Incluir (tipo de café)</t>
+  </si>
+  <si>
+    <t>ID do lote é importante?</t>
+  </si>
+  <si>
+    <t>moinho é importante?</t>
+  </si>
+  <si>
+    <t>ID do café é importante?</t>
+  </si>
+  <si>
+    <t>Nome do dono influencia?</t>
+  </si>
+  <si>
+    <t>Companhia influencia?</t>
+  </si>
+  <si>
+    <t>Objetivo :agrupar os cafés em grupo de qualidade similar</t>
+  </si>
+  <si>
+    <t>Objetivo: Prever qual será o rating do café a partir da qualidade do café (regressão linear, XGboosting, Redes Neurais)</t>
+  </si>
+  <si>
+    <t>Importante, mas o número de missing values é alto (&gt;10%) e está em intervalo</t>
+  </si>
+  <si>
+    <t>A região influencia? Já não está nos itens da qualidade?</t>
+  </si>
+  <si>
+    <t>Origem influencia? Já não está nos itens da qualidade?</t>
+  </si>
+  <si>
+    <t>Nome do torrador influencia?</t>
+  </si>
+  <si>
+    <t>Pesquisar mais sobre se o número de sacas testadas. Mas, um número maior de sacas pode significar uma maior acurácia no teste (maior amostra).</t>
+  </si>
+  <si>
+    <t>Pesquisar mais sobre se o peso de sacas testadas. Mas, um maior peso de saca pode significar uma maior acurácia no teste (maior amostra). Tratar essa coluna, pois há dados em kg e libras</t>
+  </si>
+  <si>
+    <t>Nome da fazenda influencia?</t>
+  </si>
+  <si>
+    <t>Parece importante. Número de valores únicos não muito alto (8). Transforma em dummy?</t>
+  </si>
+  <si>
+    <t>Incluir (qualidade)</t>
+  </si>
+  <si>
+    <t>Parece importante. Número de valores únicos não muito alto (5). Transforma em dummy?</t>
+  </si>
+  <si>
+    <t>Info do certificador influencia?</t>
+  </si>
+  <si>
+    <t>Medida influencia?</t>
+  </si>
+  <si>
+    <t>Data do vencimento influencia? Não seria melhor transformar em dias para o vencimento? Não temos a data de realização do teste</t>
+  </si>
+  <si>
+    <t>Altitude influencia? Já não está nos itens da qualidade?</t>
   </si>
 </sst>
 </file>
@@ -330,10 +528,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -381,16 +579,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>234315</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>127635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>272415</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -405,8 +603,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5021580" y="1821180"/>
-          <a:ext cx="4899660" cy="2308860"/>
+          <a:off x="12578715" y="2032635"/>
+          <a:ext cx="4762500" cy="2407920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -859,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86E8862-2465-4932-9384-C94448F29E51}">
   <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,8 +1066,8 @@
     <col min="1" max="1" width="44.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="26" width="8.85546875" style="1"/>
     <col min="27" max="27" width="9.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="28" max="16384" width="8.85546875" style="1"/>
@@ -890,7 +1088,7 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="AA2" s="1" t="s">
@@ -923,13 +1121,17 @@
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <v>1339</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -938,6 +1140,9 @@
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -946,13 +1151,16 @@
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -964,393 +1172,740 @@
       <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="D11" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="C14" s="2">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="2">
+        <v>359</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1063</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="2">
+        <v>315</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="2">
+        <v>151</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="2">
+        <v>209</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="2">
+        <v>226</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="2">
+        <v>59</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="2">
+        <v>231</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="2">
+        <v>47</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="2">
+        <v>7</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B30" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="2">
+        <v>226</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="2">
+        <v>170</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="B36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B39" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="B40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="B41" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="B42" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="B43" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="B44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="2"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="B45" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="2">
+        <v>218</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="B46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="B47" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="B48" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="B49" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="B50" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="B51" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="B52" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="2">
+        <v>230</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="B53" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="2">
+        <v>230</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" s="2"/>
+      <c r="C54" s="2">
+        <v>230</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update Projeto Final - Entrega 1.xlsx
Comentarios das variaveis e campo de objetivo preenchido
</commit_message>
<xml_diff>
--- a/Projeto Final - Entrega 1.xlsx
+++ b/Projeto Final - Entrega 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavio\Dropbox\My PC (LAPTOP-FVTATBSD)\Documents\Pós Insper Data Science\AEM II\Projeto Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavio\Dropbox\My PC (LAPTOP-FVTATBSD)\Documents\GitHub\TrabalhoFinalAEM2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC33597-27FC-427D-B6F5-7ECA5558D5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F472E892-852F-4751-A46F-EC0A2180B188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38578D12-16BC-486B-9148-65477D577933}"/>
   </bookViews>
@@ -383,9 +383,6 @@
     <t>Companhia influencia?</t>
   </si>
   <si>
-    <t>Objetivo :agrupar os cafés em grupo de qualidade similar</t>
-  </si>
-  <si>
     <t>Objetivo: Prever qual será o rating do café a partir da qualidade do café (regressão linear, XGboosting, Redes Neurais)</t>
   </si>
   <si>
@@ -429,6 +426,9 @@
   </si>
   <si>
     <t>Altitude influencia? Já não está nos itens da qualidade?</t>
+  </si>
+  <si>
+    <t>Objetivo :agrupar os cafés em grupo de qualidade similar.</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86E8862-2465-4932-9384-C94448F29E51}">
   <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52:E54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,7 +1141,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -1241,7 +1241,7 @@
         <v>69</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -1258,7 +1258,7 @@
         <v>70</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1343,7 +1343,7 @@
         <v>75</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
         <v>76</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1377,7 +1377,7 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1394,7 +1394,7 @@
         <v>78</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1411,7 +1411,7 @@
         <v>79</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1428,7 +1428,7 @@
         <v>80</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1445,7 +1445,7 @@
         <v>81</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
         <v>82</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1496,7 +1496,7 @@
         <v>84</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1513,7 +1513,7 @@
         <v>85</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1530,7 +1530,7 @@
         <v>86</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
         <v>87</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
         <v>88</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1581,7 +1581,7 @@
         <v>89</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1598,7 +1598,7 @@
         <v>90</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1615,7 +1615,7 @@
         <v>91</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1632,7 +1632,7 @@
         <v>92</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1649,7 +1649,7 @@
         <v>93</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1666,7 +1666,7 @@
         <v>94</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1683,7 +1683,7 @@
         <v>95</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1700,7 +1700,7 @@
         <v>96</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1717,7 +1717,7 @@
         <v>97</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1734,7 +1734,7 @@
         <v>51</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>98</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1768,7 +1768,7 @@
         <v>99</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1785,7 +1785,7 @@
         <v>100</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1802,7 +1802,7 @@
         <v>101</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1819,7 +1819,7 @@
         <v>102</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1836,7 +1836,7 @@
         <v>103</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1853,7 +1853,7 @@
         <v>104</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1870,7 +1870,7 @@
         <v>105</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1887,7 +1887,7 @@
         <v>106</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1904,7 +1904,7 @@
         <v>107</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inseridas as infos para a apresentação do dia 21
Inseridas as infos para a apresentação do dia 21
</commit_message>
<xml_diff>
--- a/Projeto Final - Entrega 1.xlsx
+++ b/Projeto Final - Entrega 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavio\Dropbox\My PC (LAPTOP-FVTATBSD)\Documents\Pós Insper Data Science\AEM II\Projeto Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavio\Dropbox\My PC (LAPTOP-FVTATBSD)\Documents\GitHub\TrabalhoFinalAEM2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C98F88B-841B-4A50-A4D9-D7D176A7CD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E044ACF-FE49-4B8F-950A-AE02AC1EC1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38578D12-16BC-486B-9148-65477D577933}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="134">
   <si>
     <t>Nome da base de dados</t>
   </si>
@@ -95,18 +95,9 @@
     <t>https://raw.githubusercontent.com/rfordatascience/tidytuesday/master/data/2020/2020-07-07/coffee_ratings.csv</t>
   </si>
   <si>
-    <t>Prever o score da avaliação do café (total_cup_points) a partir das demais preditoras do dataset e agrupar os tipos de café (cluster)</t>
-  </si>
-  <si>
-    <t>double</t>
-  </si>
-  <si>
     <t>species</t>
   </si>
   <si>
-    <t>character</t>
-  </si>
-  <si>
     <t>owner</t>
   </si>
   <si>
@@ -231,6 +222,222 @@
   </si>
   <si>
     <t>total_cup_points</t>
+  </si>
+  <si>
+    <t>dbl</t>
+  </si>
+  <si>
+    <t>chr</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Total rating/points (0 - 100 scale)</t>
+  </si>
+  <si>
+    <t>Species of coffee bean (arabica or robusta)</t>
+  </si>
+  <si>
+    <t>Owner of the farm</t>
+  </si>
+  <si>
+    <t>Where the bean came from</t>
+  </si>
+  <si>
+    <t>Name of the farm</t>
+  </si>
+  <si>
+    <t>Lot number of the beans tested</t>
+  </si>
+  <si>
+    <t>Mill where the beans were processed</t>
+  </si>
+  <si>
+    <t>International Coffee Organization number</t>
+  </si>
+  <si>
+    <t>Company name</t>
+  </si>
+  <si>
+    <t>Altitude - this is a messy column - I've left it for some cleaning</t>
+  </si>
+  <si>
+    <t>Region where bean came from</t>
+  </si>
+  <si>
+    <t>Producer of the roasted bean</t>
+  </si>
+  <si>
+    <t>Number of bags tested</t>
+  </si>
+  <si>
+    <t>Bag weight tested</t>
+  </si>
+  <si>
+    <t>Partner for the country</t>
+  </si>
+  <si>
+    <t>When the beans were harvested (year)</t>
+  </si>
+  <si>
+    <t>When the beans were graded</t>
+  </si>
+  <si>
+    <t>Who owns the beans</t>
+  </si>
+  <si>
+    <t>Variety of the beans</t>
+  </si>
+  <si>
+    <t>Method for processing</t>
+  </si>
+  <si>
+    <t>Aroma grade</t>
+  </si>
+  <si>
+    <t>Flavor grade</t>
+  </si>
+  <si>
+    <t>Aftertaste grade</t>
+  </si>
+  <si>
+    <t>Acidity grade</t>
+  </si>
+  <si>
+    <t>Body grade</t>
+  </si>
+  <si>
+    <t>Balance grade</t>
+  </si>
+  <si>
+    <t>Uniformity grade</t>
+  </si>
+  <si>
+    <t>Clean cup grade</t>
+  </si>
+  <si>
+    <t>Sweetness grade</t>
+  </si>
+  <si>
+    <t>Cupper Points</t>
+  </si>
+  <si>
+    <t>Moisture Grade</t>
+  </si>
+  <si>
+    <t>Category one defects (count)</t>
+  </si>
+  <si>
+    <t>Color of bean</t>
+  </si>
+  <si>
+    <t>Category two defects (count)</t>
+  </si>
+  <si>
+    <t>Expiration date of the beans</t>
+  </si>
+  <si>
+    <t>Who certified it</t>
+  </si>
+  <si>
+    <t>Certification body address</t>
+  </si>
+  <si>
+    <t>Certification contact</t>
+  </si>
+  <si>
+    <t>Unit of measurement</t>
+  </si>
+  <si>
+    <t>Altitude low meters</t>
+  </si>
+  <si>
+    <t>Altitude high meters</t>
+  </si>
+  <si>
+    <t>Altitude mean meters</t>
+  </si>
+  <si>
+    <t>Incluir (tipo de café)</t>
+  </si>
+  <si>
+    <t>ID do lote é importante?</t>
+  </si>
+  <si>
+    <t>moinho é importante?</t>
+  </si>
+  <si>
+    <t>ID do café é importante?</t>
+  </si>
+  <si>
+    <t>Nome do dono influencia?</t>
+  </si>
+  <si>
+    <t>Companhia influencia?</t>
+  </si>
+  <si>
+    <t>Objetivo: Prever qual será o rating do café a partir da qualidade do café (regressão linear, XGboosting, Redes Neurais)</t>
+  </si>
+  <si>
+    <t>Importante, mas o número de missing values é alto (&gt;10%) e está em intervalo</t>
+  </si>
+  <si>
+    <t>A região influencia? Já não está nos itens da qualidade?</t>
+  </si>
+  <si>
+    <t>Origem influencia? Já não está nos itens da qualidade?</t>
+  </si>
+  <si>
+    <t>Nome do torrador influencia?</t>
+  </si>
+  <si>
+    <t>Nome da fazenda influencia?</t>
+  </si>
+  <si>
+    <t>Incluir (qualidade)</t>
+  </si>
+  <si>
+    <t>Info do certificador influencia?</t>
+  </si>
+  <si>
+    <t>Data do vencimento influencia? Não seria melhor transformar em dias para o vencimento? Não temos a data de realização do teste</t>
+  </si>
+  <si>
+    <t>Altitude influencia? Já não está nos itens da qualidade?</t>
+  </si>
+  <si>
+    <t>Prever o score da avaliação do café (total_cup_points) a partir das demais preditoras do dataset e agrupar os tipos de café (cluster) a partir da qualidade do café</t>
+  </si>
+  <si>
+    <t>Objetivo :agrupar os cafés em grupo de qualidade similar a partir dos modelos de K-means e PCA.</t>
+  </si>
+  <si>
+    <t>Variável resposta</t>
+  </si>
+  <si>
+    <t>Manter e tratar considerando somente 4 regiões principais e outros</t>
+  </si>
+  <si>
+    <t>Retirar, pois não influencia no objetivo do projeto</t>
+  </si>
+  <si>
+    <t>Quando influencia? Já não está nos itens da qualidade?</t>
+  </si>
+  <si>
+    <t>Número de NA elevado</t>
+  </si>
+  <si>
+    <t>Manter e considerar os NA como Washed / Wet</t>
+  </si>
+  <si>
+    <t>Manter e considerar os NA como Green</t>
+  </si>
+  <si>
+    <t>Manter para converter as altitudes para metros</t>
+  </si>
+  <si>
+    <t>Manter e substituir os NA pela média por país</t>
   </si>
 </sst>
 </file>
@@ -262,7 +469,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,6 +485,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -330,10 +549,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -381,16 +602,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>234315</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>127635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>272415</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -405,8 +626,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5021580" y="1821180"/>
-          <a:ext cx="4899660" cy="2308860"/>
+          <a:off x="12578715" y="2032635"/>
+          <a:ext cx="4762500" cy="2407920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -860,7 +1081,7 @@
   <dimension ref="A1:AA54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,8 +1089,8 @@
     <col min="1" max="1" width="44.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="26" width="8.85546875" style="1"/>
     <col min="27" max="27" width="9.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="28" max="16384" width="8.85546875" style="1"/>
@@ -890,7 +1111,7 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="AA2" s="1" t="s">
@@ -913,7 +1134,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>4</v>
@@ -923,13 +1144,17 @@
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <v>1339</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -938,6 +1163,9 @@
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -946,13 +1174,16 @@
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -964,393 +1195,740 @@
       <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="D11" s="5" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C14" s="2">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="2">
+        <v>359</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1063</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2">
+        <v>315</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="2">
+        <v>151</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2">
+        <v>209</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2">
+        <v>226</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="2">
+        <v>59</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="2">
+        <v>231</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="2">
+        <v>47</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="2">
+        <v>7</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="2">
+        <v>226</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="2">
+        <v>170</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="B35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="B38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="B41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="B42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="B43" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="B44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="B45" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="2">
+        <v>218</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="2"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="B46" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="B47" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="B48" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="B49" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="B50" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="B51" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="B52" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="2">
+        <v>230</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="B53" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="2">
+        <v>230</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" s="2"/>
+      <c r="C54" s="2">
+        <v>230</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Ajuste no excel e ppt da apresentação
Ajustei o excel para preencher corretamente, conforme o solicitado pelos professores, e criei o ppt básico para a apresentação de amanhã.
</commit_message>
<xml_diff>
--- a/Projeto Final - Entrega 1.xlsx
+++ b/Projeto Final - Entrega 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavio\Dropbox\My PC (LAPTOP-FVTATBSD)\Documents\GitHub\TrabalhoFinalAEM2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavio\Dropbox\My PC (LAPTOP-FVTATBSD)\Documents\Pós Insper Data Science\AEM II\Projeto Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E044ACF-FE49-4B8F-950A-AE02AC1EC1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFE436F-85DE-4586-8B43-4C2D1B28CBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38578D12-16BC-486B-9148-65477D577933}"/>
   </bookViews>

</xml_diff>

<commit_message>
PPT e Excel finais
criei um novo excel (final blackboard) para subir no blackboard
</commit_message>
<xml_diff>
--- a/Projeto Final - Entrega 1.xlsx
+++ b/Projeto Final - Entrega 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavio\Dropbox\My PC (LAPTOP-FVTATBSD)\Documents\Pós Insper Data Science\AEM II\Projeto Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFE436F-85DE-4586-8B43-4C2D1B28CBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{12FE0042-FA4A-4615-A87B-3F548E3628C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38578D12-16BC-486B-9148-65477D577933}"/>
+    <workbookView xWindow="-20610" yWindow="4485" windowWidth="20730" windowHeight="11040" xr2:uid="{38578D12-16BC-486B-9148-65477D577933}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="133">
   <si>
     <t>Nome da base de dados</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Número de colunas</t>
   </si>
   <si>
-    <t>quais tratamentos fazer na base e quais modelos serão implementados</t>
-  </si>
-  <si>
     <t>Abordagem utilizada para análise supervisionada</t>
   </si>
   <si>
@@ -377,9 +374,6 @@
     <t>Companhia influencia?</t>
   </si>
   <si>
-    <t>Objetivo: Prever qual será o rating do café a partir da qualidade do café (regressão linear, XGboosting, Redes Neurais)</t>
-  </si>
-  <si>
     <t>Importante, mas o número de missing values é alto (&gt;10%) e está em intervalo</t>
   </si>
   <si>
@@ -410,9 +404,6 @@
     <t>Prever o score da avaliação do café (total_cup_points) a partir das demais preditoras do dataset e agrupar os tipos de café (cluster) a partir da qualidade do café</t>
   </si>
   <si>
-    <t>Objetivo :agrupar os cafés em grupo de qualidade similar a partir dos modelos de K-means e PCA.</t>
-  </si>
-  <si>
     <t>Variável resposta</t>
   </si>
   <si>
@@ -438,6 +429,12 @@
   </si>
   <si>
     <t>Manter e substituir os NA pela média por país</t>
+  </si>
+  <si>
+    <t>Prever qual será o rating do café a partir da qualidade do café (regressão linear, XGboosting, Redes Neurais). Para tal, serão excluídas as colunas categóricas (exceto species, country_of_origin, processing_method, color e unit_of_measurement)</t>
+  </si>
+  <si>
+    <t>Agrupar os cafés em grupo de qualidade similar a partir dos modelos de PCA e K-means. Para tal, serão excluídas as colunas categóricas (exceto species, country_of_origin, processing_method, color e unit_of_measurement)</t>
   </si>
 </sst>
 </file>
@@ -550,11 +547,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1081,7 +1078,7 @@
   <dimension ref="A1:AA54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1087,7 @@
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="57.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" style="1" customWidth="1"/>
     <col min="6" max="26" width="8.85546875" style="1"/>
     <col min="27" max="27" width="9.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="28" max="16384" width="8.85546875" style="1"/>
@@ -1101,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>6</v>
@@ -1112,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>2</v>
@@ -1134,7 +1131,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>4</v>
@@ -1158,32 +1155,26 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1196,738 +1187,738 @@
         <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C12" s="2">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>125</v>
+        <v>64</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>107</v>
+        <v>65</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2">
         <v>7</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>126</v>
+        <v>67</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="2">
         <v>359</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="2">
         <v>1063</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="2">
         <v>315</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2">
         <v>151</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="2">
         <v>209</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="2">
         <v>226</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="2">
         <v>59</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2">
         <v>231</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="2">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="2">
         <v>47</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2">
         <v>7</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="2">
         <v>226</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="2">
         <v>170</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>130</v>
+        <v>83</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>119</v>
+        <v>84</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>119</v>
+        <v>85</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="2">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>119</v>
+        <v>86</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" s="2">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>119</v>
+        <v>87</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="2">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>119</v>
+        <v>88</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37" s="2">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>119</v>
+        <v>89</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" s="2">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>119</v>
+        <v>90</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39" s="2">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>119</v>
+        <v>91</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="2">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>119</v>
+        <v>92</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C41" s="2">
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>119</v>
+        <v>93</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" s="2">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>119</v>
+        <v>94</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" s="2">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>119</v>
+        <v>95</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>119</v>
+        <v>49</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" s="2">
         <v>218</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>131</v>
+        <v>96</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="2">
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>119</v>
+        <v>97</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" s="2">
         <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" s="2">
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" s="2">
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" s="2">
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C51" s="2">
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>132</v>
+        <v>102</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" s="2">
         <v>230</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="2">
         <v>230</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" s="2">
         <v>230</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>133</v>
+        <v>105</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>